<commit_message>
1) Fixing the BOM ... dumbass
</commit_message>
<xml_diff>
--- a/Hardware/LAB-PPS330D/docs/LAB-PPS330D-Rev1BOM.xlsx
+++ b/Hardware/LAB-PPS330D/docs/LAB-PPS330D-Rev1BOM.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="13380" yWindow="-30" windowWidth="18345" windowHeight="13440"/>
+    <workbookView xWindow="15750" yWindow="-30" windowWidth="18345" windowHeight="13440"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials" sheetId="2" r:id="rId1"/>
@@ -129,12 +129,6 @@
     <t>6-SSOT</t>
   </si>
   <si>
-    <t>U2, U3</t>
-  </si>
-  <si>
-    <t>U4</t>
-  </si>
-  <si>
     <t>296-18203-1-ND</t>
   </si>
   <si>
@@ -193,6 +187,12 @@
   </si>
   <si>
     <t>1276-3484-1-ND</t>
+  </si>
+  <si>
+    <t>U3, U4</t>
+  </si>
+  <si>
+    <t>U2</t>
   </si>
 </sst>
 </file>
@@ -444,32 +444,32 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -779,7 +779,7 @@
   <dimension ref="A1:L65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -809,11 +809,11 @@
     </row>
     <row r="2" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="25"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="29"/>
       <c r="E2" s="2"/>
       <c r="F2" s="8"/>
       <c r="G2" s="2"/>
@@ -824,10 +824,10 @@
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="27"/>
+      <c r="D3" s="31"/>
       <c r="E3" s="2"/>
       <c r="F3" s="8"/>
       <c r="G3" s="2"/>
@@ -838,10 +838,10 @@
       <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="27"/>
+      <c r="D4" s="31"/>
       <c r="E4" s="2"/>
       <c r="F4" s="8"/>
       <c r="G4" s="2"/>
@@ -852,10 +852,10 @@
       <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="27"/>
+      <c r="D5" s="31"/>
       <c r="E5" s="2"/>
       <c r="F5" s="8"/>
       <c r="G5" s="2"/>
@@ -866,10 +866,10 @@
       <c r="B6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="28" t="s">
+      <c r="C6" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="29"/>
+      <c r="D6" s="33"/>
       <c r="E6" s="2"/>
       <c r="F6" s="8"/>
       <c r="G6" s="2"/>
@@ -917,10 +917,10 @@
         <v>15</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="L8" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -984,7 +984,7 @@
         <v>0.13159999999999999</v>
       </c>
       <c r="L10">
-        <f t="shared" ref="L10:L26" si="0">K10*G10</f>
+        <f t="shared" ref="L10:L15" si="0">K10*G10</f>
         <v>0.26319999999999999</v>
       </c>
     </row>
@@ -993,16 +993,16 @@
         <v>3</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C11" s="14" t="s">
         <v>13</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F11" s="15" t="s">
         <v>12</v>
@@ -1014,9 +1014,9 @@
         <v>25</v>
       </c>
       <c r="J11" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="K11" s="31">
+        <v>36</v>
+      </c>
+      <c r="K11" s="24">
         <v>0.45500000000000002</v>
       </c>
       <c r="L11">
@@ -1040,8 +1040,8 @@
       <c r="E12" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="F12" s="21" t="s">
-        <v>36</v>
+      <c r="F12" s="15" t="s">
+        <v>56</v>
       </c>
       <c r="G12" s="19">
         <v>2</v>
@@ -1051,9 +1051,9 @@
         <v>25</v>
       </c>
       <c r="J12" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="K12" s="31">
+        <v>37</v>
+      </c>
+      <c r="K12" s="24">
         <v>0.27979999999999999</v>
       </c>
       <c r="L12">
@@ -1077,8 +1077,8 @@
       <c r="E13" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="F13" s="21" t="s">
-        <v>37</v>
+      <c r="F13" s="15" t="s">
+        <v>57</v>
       </c>
       <c r="G13" s="19">
         <v>1</v>
@@ -1088,9 +1088,9 @@
         <v>25</v>
       </c>
       <c r="J13" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="K13" s="31">
+        <v>38</v>
+      </c>
+      <c r="K13" s="24">
         <v>0.40060000000000001</v>
       </c>
       <c r="L13">
@@ -1103,19 +1103,19 @@
         <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="D14" s="30" t="s">
-        <v>50</v>
+        <v>40</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>48</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F14" s="21" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G14" s="19">
         <v>3</v>
@@ -1125,9 +1125,9 @@
         <v>25</v>
       </c>
       <c r="J14" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="K14" s="31">
+        <v>45</v>
+      </c>
+      <c r="K14" s="24">
         <v>0.13952000000000001</v>
       </c>
       <c r="L14">
@@ -1139,20 +1139,20 @@
       <c r="A15" s="11">
         <v>7</v>
       </c>
-      <c r="B15" s="33" t="s">
+      <c r="B15" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="C15" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="D15" s="31" t="s">
-        <v>56</v>
-      </c>
       <c r="E15" s="19" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F15" s="21" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G15" s="19">
         <v>1</v>
@@ -1162,9 +1162,9 @@
         <v>25</v>
       </c>
       <c r="J15" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="K15" s="31">
+        <v>55</v>
+      </c>
+      <c r="K15" s="24">
         <v>3.48E-3</v>
       </c>
       <c r="L15">
@@ -1173,10 +1173,10 @@
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K16" s="32" t="s">
-        <v>53</v>
-      </c>
-      <c r="L16" s="32">
+      <c r="K16" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="L16" s="25">
         <f>SUM(L9:L15)</f>
         <v>2.8423400000000005</v>
       </c>
@@ -1188,7 +1188,7 @@
       <c r="E17" s="14"/>
       <c r="F17" s="15"/>
       <c r="G17" s="14"/>
-      <c r="K17" s="31"/>
+      <c r="K17" s="24"/>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" s="16"/>
@@ -1197,7 +1197,7 @@
       <c r="E18" s="14"/>
       <c r="F18" s="15"/>
       <c r="G18" s="14"/>
-      <c r="K18" s="31"/>
+      <c r="K18" s="24"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" s="16"/>
@@ -1206,7 +1206,7 @@
       <c r="E19" s="14"/>
       <c r="F19" s="15"/>
       <c r="G19" s="14"/>
-      <c r="K19" s="31"/>
+      <c r="K19" s="24"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" s="16"/>
@@ -1215,7 +1215,7 @@
       <c r="E20" s="14"/>
       <c r="F20" s="15"/>
       <c r="G20" s="14"/>
-      <c r="K20" s="31"/>
+      <c r="K20" s="24"/>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" s="16"/>
@@ -1224,7 +1224,7 @@
       <c r="E21" s="14"/>
       <c r="F21" s="15"/>
       <c r="G21" s="14"/>
-      <c r="K21" s="31"/>
+      <c r="K21" s="24"/>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22" s="16"/>
@@ -1233,7 +1233,7 @@
       <c r="E22" s="14"/>
       <c r="F22" s="15"/>
       <c r="G22" s="14"/>
-      <c r="K22" s="31"/>
+      <c r="K22" s="24"/>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23" s="16"/>
@@ -1242,7 +1242,7 @@
       <c r="E23" s="14"/>
       <c r="F23" s="15"/>
       <c r="G23" s="14"/>
-      <c r="K23" s="31"/>
+      <c r="K23" s="24"/>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B24" s="16"/>
@@ -1251,7 +1251,7 @@
       <c r="E24" s="14"/>
       <c r="F24" s="15"/>
       <c r="G24" s="14"/>
-      <c r="K24" s="31"/>
+      <c r="K24" s="24"/>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B25" s="16"/>
@@ -1260,7 +1260,7 @@
       <c r="E25" s="14"/>
       <c r="F25" s="15"/>
       <c r="G25" s="14"/>
-      <c r="K25" s="31"/>
+      <c r="K25" s="24"/>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B26" s="16"/>
@@ -1269,7 +1269,7 @@
       <c r="E26" s="14"/>
       <c r="F26" s="15"/>
       <c r="G26" s="14"/>
-      <c r="K26" s="31"/>
+      <c r="K26" s="24"/>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B27" s="16"/>

</xml_diff>